<commit_message>
update fix narasumber, honorarium dan formulir kelas
</commit_message>
<xml_diff>
--- a/docs/template-excel/narasumber.xlsx
+++ b/docs/template-excel/narasumber.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\Proyek-Honorarium\dokumen-upload\template excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FATHUR\KERJAAN\Proyek-Honorarium\source-code\honorarium\docs\template-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28476C61-0181-402B-B751-5E1820872814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC18DE0A-A2FD-483F-94F5-8DFF4883BAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{674168BC-6BCF-C342-9E35-C2DEB8BAE251}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>ID</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>33333</t>
-  </si>
-  <si>
-    <t>II</t>
   </si>
   <si>
     <t>Kepala Pusdiklat</t>
@@ -269,7 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +602,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -628,13 +625,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -649,17 +646,17 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="N1" s="5"/>
       <c r="P1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -679,26 +676,26 @@
         <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -718,28 +715,28 @@
         <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -757,96 +754,96 @@
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2" t="s">
         <v>9</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="P4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>